<commit_message>
adding dates to templates
</commit_message>
<xml_diff>
--- a/assets/modules/seagrass-quadrats/MarineGEO_Seagrass-Quadrat_DataEntryTemplate_v0.0.1.xlsx
+++ b/assets/modules/seagrass-quadrats/MarineGEO_Seagrass-Quadrat_DataEntryTemplate_v0.0.1.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11015"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ambell/Documents/MarineGEO-template-workbooks/seagrass-quadrats/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B2FF89-35BE-664C-9B05-F86EBD0BEA0E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="22840" windowHeight="16360" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -28,17 +22,17 @@
     <definedName name="site">Vocab!$B$9:$B$20</definedName>
     <definedName name="taxonRank">Vocab!$B$2:$B$8</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="B4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -51,7 +45,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -64,7 +58,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="B6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -77,7 +71,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="B7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -90,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="B8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -103,7 +97,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="B9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -116,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="B10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -129,7 +123,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="B11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -142,7 +136,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="B12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -155,7 +149,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="B13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -168,7 +162,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="B14" authorId="0">
       <text>
         <r>
           <rPr>
@@ -186,7 +180,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="171">
   <si>
     <t>MarineGEO Seagrass Shoots Template</t>
   </si>
@@ -230,7 +224,7 @@
     <t>WorkbookBuildInfo</t>
   </si>
   <si>
-    <t>Created using MarinegeoTemplateBuilder v0.1.7 on 2018-11-08 15:57</t>
+    <t>Created using MarinegeoTemplateBuilder v0.1.7 on 2018-11-08 16:43</t>
   </si>
   <si>
     <t>site</t>
@@ -242,15 +236,15 @@
     <t>locality</t>
   </si>
   <si>
+    <t>date</t>
+  </si>
+  <si>
     <t>decimalLatitude</t>
   </si>
   <si>
     <t>decimalLongitude</t>
   </si>
   <si>
-    <t>habitat</t>
-  </si>
-  <si>
     <t>locationRemarks</t>
   </si>
   <si>
@@ -593,9 +587,6 @@
     <t>Date the data was entered to this form. If data was entered over multiple days, please report the last date.</t>
   </si>
   <si>
-    <t>date</t>
-  </si>
-  <si>
     <t>YYYY-MM-DD</t>
   </si>
   <si>
@@ -623,6 +614,9 @@
     <t>Local or common name of the sampling location</t>
   </si>
   <si>
+    <t>Sampling date</t>
+  </si>
+  <si>
     <t>Decimal latitude hh.hhhhhhh</t>
   </si>
   <si>
@@ -633,9 +627,6 @@
   </si>
   <si>
     <t>Decimal longitude hh.hhhhhhh</t>
-  </si>
-  <si>
-    <t>habitat type at sampling location</t>
   </si>
   <si>
     <t>Comments or notes about the location</t>
@@ -707,17 +698,24 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -749,12 +747,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -798,19 +790,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -830,14 +824,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -858,13 +844,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="marinegeo_branding.png">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="marinegeo_branding.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -933,7 +913,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -965,27 +945,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1017,24 +979,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1210,96 +1154,96 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FF97C8EB"/>
   </sheetPr>
   <dimension ref="A3:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="40" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="40" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="40.6640625" customWidth="1"/>
-    <col min="2" max="2" width="100.6640625" customWidth="1"/>
+    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="2" max="2" width="100.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" ht="40" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:2" ht="40" customHeight="1">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:2" ht="40" customHeight="1">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="80" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:2" ht="80" customHeight="1">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3"/>
-    </row>
-    <row r="6" spans="1:2" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="B5" s="4"/>
+    </row>
+    <row r="6" spans="1:2" ht="40" customHeight="1">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:2" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="B6" s="4"/>
+    </row>
+    <row r="7" spans="1:2" ht="40" customHeight="1">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3"/>
-    </row>
-    <row r="8" spans="1:2" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:2" ht="40" customHeight="1">
+      <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3"/>
-    </row>
-    <row r="9" spans="1:2" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="1:2" ht="40" customHeight="1">
+      <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="3"/>
-    </row>
-    <row r="10" spans="1:2" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" spans="1:2" ht="40" customHeight="1">
+      <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="4"/>
-    </row>
-    <row r="11" spans="1:2" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="B10" s="5"/>
+    </row>
+    <row r="11" spans="1:2" ht="40" customHeight="1">
+      <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="3"/>
-    </row>
-    <row r="12" spans="1:2" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="B11" s="4"/>
+    </row>
+    <row r="12" spans="1:2" ht="40" customHeight="1">
+      <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:2" ht="40" customHeight="1">
+      <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:2" ht="40" customHeight="1">
+      <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1310,7 +1254,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10">
       <formula1>-693594</formula1>
     </dataValidation>
   </dataValidations>
@@ -1321,7 +1265,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FF97C8EB"/>
   </sheetPr>
@@ -1332,46 +1276,50 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="8" width="18.6640625" customWidth="1"/>
+    <col min="1" max="8" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="7" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A20001" xr:uid="{00000000-0002-0000-0100-000000000000}">
+  <dataValidations count="4">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A20001">
       <formula1>site</formula1>
     </dataValidation>
-    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Decimal must be between -90.0 and 90.0." sqref="D2:D20001" xr:uid="{00000000-0002-0000-0100-000001000000}">
-      <formula1>-90</formula1>
-      <formula2>90</formula2>
+    <dataValidation type="date" operator="greaterThan" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D20001">
+      <formula1>-693594</formula1>
     </dataValidation>
-    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Decimal must be between -180.0 and 180.0." sqref="E2:E20001" xr:uid="{00000000-0002-0000-0100-000002000000}">
-      <formula1>-180</formula1>
-      <formula2>180</formula2>
+    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Decimal must be between -90.0 and 90.0." sqref="E2:E20001">
+      <formula1>-90.0</formula1>
+      <formula2>90.0</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Decimal must be between -180.0 and 180.0." sqref="F2:F20001">
+      <formula1>-180.0</formula1>
+      <formula2>180.0</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1379,7 +1327,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FF97C8EB"/>
   </sheetPr>
@@ -1390,66 +1338,57 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="7" width="18.6640625" customWidth="1"/>
+    <col min="1" max="7" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="7" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Integer must be between 1.0 and 3.0." sqref="B2:B20001" xr:uid="{00000000-0002-0000-0200-000001000000}">
-      <formula1>1</formula1>
-      <formula2>3</formula2>
+  <dataValidations count="5">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A20001">
+      <formula1>OFFSET(Location!$B:$B, 1, 0, ROWS(Location!$B:$B)-1)</formula1>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Integer must be between 1.0 and 12.0." sqref="C2:C20001" xr:uid="{00000000-0002-0000-0200-000002000000}">
-      <formula1>1</formula1>
-      <formula2>12</formula2>
+    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Integer must be between 1.0 and 3.0." sqref="B2:B20001">
+      <formula1>1.0</formula1>
+      <formula2>3.0</formula2>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D20001" xr:uid="{00000000-0002-0000-0200-000003000000}">
+    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Integer must be between 1.0 and 12.0." sqref="C2:C20001">
+      <formula1>1.0</formula1>
+      <formula2>12.0</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D20001">
       <formula1>coverType</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F20001" xr:uid="{00000000-0002-0000-0200-000004000000}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F20001">
       <formula1>percentCover</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
-          <x14:formula1>
-            <xm:f>OFFSET(Location!$B:$B, 1, 0, ROWS(Location!$B:$B)-1)</xm:f>
-          </x14:formula1>
-          <xm:sqref>A2:A20001</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FF97C8EB"/>
   </sheetPr>
@@ -1460,142 +1399,124 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="7" width="18.6640625" customWidth="1"/>
+    <col min="1" max="7" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="7" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Integer must be between 1.0 and 3.0." sqref="B2:B20001" xr:uid="{00000000-0002-0000-0300-000001000000}">
-      <formula1>1</formula1>
-      <formula2>3</formula2>
+  <dataValidations count="5">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A20001">
+      <formula1>OFFSET(Location!$B:$B, 1, 0, ROWS(Location!$B:$B)-1)</formula1>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Integer must be between 1.0 and 12.0." sqref="C2:C20001" xr:uid="{00000000-0002-0000-0300-000002000000}">
-      <formula1>1</formula1>
-      <formula2>12</formula2>
+    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Integer must be between 1.0 and 3.0." sqref="B2:B20001">
+      <formula1>1.0</formula1>
+      <formula2>3.0</formula2>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Integer must be greater than 0.0." sqref="D2:D20001" xr:uid="{00000000-0002-0000-0300-000003000000}">
-      <formula1>0</formula1>
+    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Integer must be between 1.0 and 12.0." sqref="C2:C20001">
+      <formula1>1.0</formula1>
+      <formula2>12.0</formula2>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E20001" xr:uid="{00000000-0002-0000-0300-000004000000}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Integer must be greater than 0.0." sqref="D2:D20001">
+      <formula1>0.0</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E20001">
       <formula1>grazingScars</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000000000000}">
-          <x14:formula1>
-            <xm:f>OFFSET(Location!$B:$B, 1, 0, ROWS(Location!$B:$B)-1)</xm:f>
-          </x14:formula1>
-          <xm:sqref>A2:A20001</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FF97C8EB"/>
   </sheetPr>
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="9" width="18.6640625" customWidth="1"/>
+    <col min="1" max="9" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="7" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Integer must be between 1.0 and 3.0." sqref="B2:B20001" xr:uid="{00000000-0002-0000-0400-000001000000}">
-      <formula1>1</formula1>
-      <formula2>3</formula2>
+  <dataValidations count="5">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A20001">
+      <formula1>OFFSET(Location!$B:$B, 1, 0, ROWS(Location!$B:$B)-1)</formula1>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Integer must be between 1.0 and 12.0." sqref="C2:C20001" xr:uid="{00000000-0002-0000-0400-000002000000}">
-      <formula1>1</formula1>
-      <formula2>12</formula2>
+    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Integer must be between 1.0 and 3.0." sqref="B2:B20001">
+      <formula1>1.0</formula1>
+      <formula2>3.0</formula2>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E20001" xr:uid="{00000000-0002-0000-0400-000003000000}">
+    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Integer must be between 1.0 and 12.0." sqref="C2:C20001">
+      <formula1>1.0</formula1>
+      <formula2>12.0</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E20001">
       <formula1>taxonRank</formula1>
     </dataValidation>
-    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Decimal must be greater than 0.0." sqref="H2:H20001" xr:uid="{00000000-0002-0000-0400-000004000000}">
-      <formula1>0</formula1>
+    <dataValidation type="decimal" operator="greaterThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Decimal must be greater than 0.0." sqref="H2:H20001">
+      <formula1>0.0</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000000000000}">
-          <x14:formula1>
-            <xm:f>OFFSET(Location!$B:$B, 1, 0, ROWS(Location!$B:$B)-1)</xm:f>
-          </x14:formula1>
-          <xm:sqref>A2:A20001</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FF97C8EB"/>
   </sheetPr>
@@ -1606,495 +1527,494 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="40.6640625" customWidth="1"/>
-    <col min="3" max="3" width="100.6640625" customWidth="1"/>
-    <col min="4" max="4" width="40.6640625" customWidth="1"/>
+    <col min="1" max="4" width="40.7109375" customWidth="1"/>
+    <col min="3" max="3" width="100.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:3">
+      <c r="A2" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:3">
+      <c r="A3" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:3">
+      <c r="A4" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:3">
+      <c r="A5" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:3">
+      <c r="A6" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:3">
+      <c r="A7" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:3">
+      <c r="A8" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:3">
+      <c r="A9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:3">
+      <c r="A10" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:3">
+      <c r="A11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:3">
+      <c r="A12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:3">
+      <c r="A13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:3">
+      <c r="A14" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:3">
+      <c r="A15" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+    <row r="16" spans="1:3">
+      <c r="A16" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+    <row r="17" spans="1:3">
+      <c r="A17" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+    <row r="18" spans="1:3">
+      <c r="A18" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
+    <row r="19" spans="1:3">
+      <c r="A19" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="8" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+    <row r="20" spans="1:3">
+      <c r="A20" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="8" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
+    <row r="21" spans="1:3">
+      <c r="A21" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="8" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
+    <row r="22" spans="1:3">
+      <c r="A22" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="8" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
+    <row r="23" spans="1:3">
+      <c r="A23" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="8" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
+    <row r="24" spans="1:3">
+      <c r="A24" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
+    <row r="25" spans="1:3">
+      <c r="A25" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="s">
+    <row r="26" spans="1:3">
+      <c r="A26" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="8" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="6" t="s">
+    <row r="27" spans="1:3">
+      <c r="A27" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="8" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
+    <row r="28" spans="1:3">
+      <c r="A28" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="s">
+    <row r="29" spans="1:3">
+      <c r="A29" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="6" t="s">
+    <row r="30" spans="1:3">
+      <c r="A30" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="6" t="s">
+    <row r="31" spans="1:3">
+      <c r="A31" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="8" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="6" t="s">
+    <row r="32" spans="1:3">
+      <c r="A32" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="8" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="6" t="s">
+    <row r="33" spans="1:3">
+      <c r="A33" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="8" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="6" t="s">
+    <row r="34" spans="1:3">
+      <c r="A34" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="8" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" s="6" t="s">
+    <row r="35" spans="1:3">
+      <c r="A35" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="8" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" s="6" t="s">
+    <row r="36" spans="1:3">
+      <c r="A36" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="8" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="6" t="s">
+    <row r="37" spans="1:3">
+      <c r="A37" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="8" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="6" t="s">
+    <row r="38" spans="1:3">
+      <c r="A38" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="8" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A39" s="6" t="s">
+    <row r="39" spans="1:3">
+      <c r="A39" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="8" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" s="6" t="s">
+    <row r="40" spans="1:3">
+      <c r="A40" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C40" s="8" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" s="6" t="s">
+    <row r="41" spans="1:3">
+      <c r="A41" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C41" s="8" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="6" t="s">
+    <row r="42" spans="1:3">
+      <c r="A42" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C42" s="8" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" s="6" t="s">
+    <row r="43" spans="1:3">
+      <c r="A43" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="8" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" s="6" t="s">
+    <row r="44" spans="1:3">
+      <c r="A44" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C44" s="8" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A45" s="6" t="s">
+    <row r="45" spans="1:3">
+      <c r="A45" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C45" s="8" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="6" t="s">
+    <row r="46" spans="1:3">
+      <c r="A46" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C46" s="8" t="s">
         <v>120</v>
       </c>
     </row>
@@ -2105,7 +2025,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FF97C8EB"/>
   </sheetPr>
@@ -2116,594 +2036,597 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="50" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="50" customHeight="1"/>
   <cols>
-    <col min="1" max="3" width="40.6640625" customWidth="1"/>
-    <col min="4" max="7" width="18.6640625" customWidth="1"/>
+    <col min="1" max="3" width="40.7109375" customWidth="1"/>
+    <col min="4" max="7" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:6" ht="50" customHeight="1">
+      <c r="A1" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="7" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:6" ht="50" customHeight="1">
+      <c r="A2" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="8" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:6" ht="50" customHeight="1">
+      <c r="A3" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="8" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:6" ht="50" customHeight="1">
+      <c r="A4" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="8" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:6" ht="50" customHeight="1">
+      <c r="A5" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="8" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:6" ht="50" customHeight="1">
+      <c r="A6" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="8" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:6" ht="50" customHeight="1">
+      <c r="A7" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="8" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:6" ht="50" customHeight="1">
+      <c r="A8" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="E8" s="6" t="s">
+    </row>
+    <row r="9" spans="1:6" ht="50" customHeight="1">
+      <c r="A9" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+      <c r="D9" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="50" customHeight="1">
+      <c r="A10" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="B10" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D10" s="8" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+    <row r="11" spans="1:6" ht="50" customHeight="1">
+      <c r="A11" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="6" t="s">
+      <c r="B11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D11" s="8" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+    <row r="12" spans="1:6" ht="50" customHeight="1">
+      <c r="A12" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="50" customHeight="1">
+      <c r="A13" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="50" customHeight="1">
+      <c r="A14" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="50" customHeight="1">
+      <c r="A15" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="50" customHeight="1">
+      <c r="A16" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="50" customHeight="1">
+      <c r="A17" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="50" customHeight="1">
+      <c r="A18" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="50" customHeight="1">
+      <c r="A19" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="50" customHeight="1">
+      <c r="A20" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="50" customHeight="1">
+      <c r="A21" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="50" customHeight="1">
+      <c r="A22" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="50" customHeight="1">
+      <c r="A23" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="50" customHeight="1">
+      <c r="A24" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="50" customHeight="1">
+      <c r="A25" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="50" customHeight="1">
+      <c r="A26" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="50" customHeight="1">
+      <c r="A27" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="50" customHeight="1">
+      <c r="A28" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="50" customHeight="1">
+      <c r="A29" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="50" customHeight="1">
+      <c r="A30" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="50" customHeight="1">
+      <c r="A31" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="50" customHeight="1">
+      <c r="A32" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="50" customHeight="1">
+      <c r="A33" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="50" customHeight="1">
+      <c r="A34" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="50" customHeight="1">
+      <c r="A35" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="50" customHeight="1">
+      <c r="A36" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="50" customHeight="1">
+      <c r="A37" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="50" customHeight="1">
+      <c r="A38" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="50" customHeight="1">
+      <c r="A39" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="F38" s="6" t="s">
+      <c r="B39" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="8" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="D39" s="6" t="s">
+      <c r="D39" s="8" t="s">
         <v>128</v>
       </c>
     </row>

</xml_diff>

<commit_message>
seagrass shoot protocol, sheets
</commit_message>
<xml_diff>
--- a/assets/modules/seagrass-quadrats/MarineGEO_Seagrass-Quadrat_DataEntryTemplate_v0.0.1.xlsx
+++ b/assets/modules/seagrass-quadrats/MarineGEO_Seagrass-Quadrat_DataEntryTemplate_v0.0.1.xlsx
@@ -26,159 +26,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment ref="B4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="16"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Brief unique name describing location, type of data collected and dates</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="16"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Short description that contains details about what, why, how, when, and where the data was collected</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B6" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="16"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Full name of data set creator (First Last). One person only.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B7" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="16"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Email address for data set creator</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B8" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="16"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Full names of all people that collected data. Separate multiple names with semicolons (ie Person One; Person Two; Person Three)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B9" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="16"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Full name of person(s) entering data. Separate multiple names with semicolons.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B10" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="16"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Date the data was entered to this form. If data was entered over multiple days, please report the last date.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B11" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="16"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>General notes about the project</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B12" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="16"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Protocol version number if applicable</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B13" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="16"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Data template spreadsheet version</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B14" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="16"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Information about the tool used to create the excel template</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="171">
   <si>
@@ -224,7 +71,7 @@
     <t>WorkbookBuildInfo</t>
   </si>
   <si>
-    <t>Created using MarinegeoTemplateBuilder v0.1.7 on 2018-11-08 16:43</t>
+    <t>Created using MarinegeoTemplateBuilder v0.1.8 on 2018-11-09 11:16</t>
   </si>
   <si>
     <t>site</t>
@@ -703,19 +550,13 @@
     <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
     <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -790,21 +631,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1169,81 +1009,81 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:2" ht="40" customHeight="1">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="40" customHeight="1">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="80" customHeight="1">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="3"/>
     </row>
     <row r="6" spans="1:2" ht="40" customHeight="1">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="3"/>
     </row>
     <row r="7" spans="1:2" ht="40" customHeight="1">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:2" ht="40" customHeight="1">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="3"/>
     </row>
     <row r="9" spans="1:2" ht="40" customHeight="1">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4"/>
+      <c r="B9" s="3"/>
     </row>
     <row r="10" spans="1:2" ht="40" customHeight="1">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="5"/>
+      <c r="B10" s="4"/>
     </row>
     <row r="11" spans="1:2" ht="40" customHeight="1">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:2" ht="40" customHeight="1">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="40" customHeight="1">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="40" customHeight="1">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1260,7 +1100,6 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1279,29 +1118,29 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="8" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1344,22 +1183,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1405,22 +1244,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1466,28 +1305,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1534,487 +1373,487 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="7" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="7" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="7" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="7" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="7" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="7" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="7" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="7" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="7" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="7" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="7" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="7" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="7" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="8" t="s">
+      <c r="A33" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="7" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="7" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="8" t="s">
+      <c r="A35" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="7" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="7" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="7" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="8" t="s">
+      <c r="A38" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C38" s="7" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="8" t="s">
+      <c r="A39" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="7" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="8" t="s">
+      <c r="A40" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B40" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C40" s="7" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="8" t="s">
+      <c r="A41" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="B41" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="C41" s="7" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="8" t="s">
+      <c r="A42" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B42" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="C42" s="7" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B43" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C43" s="7" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="8" t="s">
+      <c r="A44" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="B44" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="C44" s="7" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="8" t="s">
+      <c r="A45" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B45" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="C45" s="7" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="8" t="s">
+      <c r="A46" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B46" s="8" t="s">
+      <c r="B46" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="C46" s="7" t="s">
         <v>120</v>
       </c>
     </row>
@@ -2043,590 +1882,590 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="50" customHeight="1">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="50" customHeight="1">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="50" customHeight="1">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="50" customHeight="1">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="50" customHeight="1">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="50" customHeight="1">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="50" customHeight="1">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="50" customHeight="1">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="7" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="50" customHeight="1">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="50" customHeight="1">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="50" customHeight="1">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="50" customHeight="1">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="7" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="50" customHeight="1">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="7" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="50" customHeight="1">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="7" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="50" customHeight="1">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="7" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="50" customHeight="1">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="7" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="50" customHeight="1">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="7" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="50" customHeight="1">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="7" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="50" customHeight="1">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="7" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="50" customHeight="1">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="7" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="50" customHeight="1">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F21" s="7" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="50" customHeight="1">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="7" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="50" customHeight="1">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="7" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="50" customHeight="1">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="7" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="50" customHeight="1">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="7" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="50" customHeight="1">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="7" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="50" customHeight="1">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="F27" s="7" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="50" customHeight="1">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="F28" s="8" t="s">
+      <c r="F28" s="7" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="50" customHeight="1">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="7" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="50" customHeight="1">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="7" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="50" customHeight="1">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="7" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="50" customHeight="1">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="F32" s="8" t="s">
+      <c r="F32" s="7" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="50" customHeight="1">
-      <c r="A33" s="8" t="s">
+      <c r="A33" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="F33" s="8" t="s">
+      <c r="F33" s="7" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="50" customHeight="1">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="7" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="50" customHeight="1">
-      <c r="A35" s="8" t="s">
+      <c r="A35" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="7" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="50" customHeight="1">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="7" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="50" customHeight="1">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D37" s="7" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="50" customHeight="1">
-      <c r="A38" s="8" t="s">
+      <c r="A38" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C38" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D38" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="F38" s="8" t="s">
+      <c r="F38" s="7" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="50" customHeight="1">
-      <c r="A39" s="8" t="s">
+      <c r="A39" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D39" s="7" t="s">
         <v>128</v>
       </c>
     </row>

</xml_diff>